<commit_message>
Always seems like more changes than are strictly necessary
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-botswana-amr-diagnostic-report.xlsx
+++ b/output/StructureDefinition-botswana-amr-diagnostic-report.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="395">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-25T00:42:48-04:00</t>
+    <t>2025-07-08T11:52:18-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Bundles AMR susceptibility observations into one report</t>
+    <t>Bundles AMR susceptibility observations into one comprehensive report</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -705,6 +705,9 @@
   </si>
   <si>
     <t>Diagnostic services routinely issue provisional/incomplete reports, and sometimes withdraw previously released reports.</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
   <si>
     <t>required</t>
@@ -807,7 +810,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient)
+    <t xml:space="preserve">Reference(http://bw.health.gov/fhir/ImplementationGuide/bw-amr-ig/StructureDefinition/botswana-amr-patient)
 </t>
   </si>
   <si>
@@ -1000,7 +1003,7 @@
     <t>DiagnosticReport.specimen</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Specimen)
+    <t xml:space="preserve">Reference(http://bw.health.gov/fhir/ImplementationGuide/bw-amr-ig/StructureDefinition/botswana-amr-specimen)
 </t>
   </si>
   <si>
@@ -1042,10 +1045,54 @@
     <t>Need to support individual results, or  groups of results, where the result grouping is arbitrary, but meaningful.</t>
   </si>
   <si>
+    <t xml:space="preserve">pattern:resolve().code}
+</t>
+  </si>
+  <si>
     <t>OBXs</t>
   </si>
   <si>
     <t>outboundRelationship[typeCode=COMP].target</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.result:gramStain</t>
+  </si>
+  <si>
+    <t>gramStain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://bw.health.gov/fhir/ImplementationGuide/bw-amr-ig/StructureDefinition/botswana-amr-gram-stain-observation)
+</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.result:organism</t>
+  </si>
+  <si>
+    <t>organism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://bw.health.gov/fhir/ImplementationGuide/bw-amr-ig/StructureDefinition/botswana-amr-organism-observation)
+</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.result:susceptibility</t>
+  </si>
+  <si>
+    <t>susceptibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://bw.health.gov/fhir/ImplementationGuide/bw-amr-ig/StructureDefinition/botswana-amr-susceptibility-observation)
+</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.result:specialTests</t>
+  </si>
+  <si>
+    <t>specialTests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://bw.health.gov/fhir/ImplementationGuide/bw-amr-ig/StructureDefinition/botswana-amr-special-test-observation)
+</t>
   </si>
   <si>
     <t>DiagnosticReport.imagingStudy</t>
@@ -1519,7 +1566,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN42"/>
+  <dimension ref="A1:AN46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1538,7 +1585,7 @@
     <col min="8" max="8" width="13.609375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.1796875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="88.17578125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="108.9453125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1555,7 +1602,7 @@
     <col min="25" max="25" width="30.55859375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="48.58203125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.2734375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.1171875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.55859375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.56640625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="14.3671875" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="11.84375" customWidth="true" bestFit="true" hidden="true"/>
@@ -3903,7 +3950,7 @@
         <v>20</v>
       </c>
       <c r="S21" t="s" s="2">
-        <v>11</v>
+        <v>222</v>
       </c>
       <c r="T21" t="s" s="2">
         <v>20</v>
@@ -3918,13 +3965,13 @@
         <v>20</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="Y21" t="s" s="2">
         <v>220</v>
       </c>
       <c r="Z21" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>20</v>
@@ -3957,28 +4004,28 @@
         <v>102</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
@@ -3997,16 +4044,16 @@
         <v>91</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
@@ -4035,10 +4082,10 @@
         <v>155</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>20</v>
@@ -4056,7 +4103,7 @@
         <v>20</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -4074,25 +4121,25 @@
         <v>20</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
@@ -4111,13 +4158,13 @@
         <v>91</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -4129,7 +4176,7 @@
         <v>20</v>
       </c>
       <c r="S23" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="T23" t="s" s="2">
         <v>20</v>
@@ -4147,10 +4194,10 @@
         <v>168</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>20</v>
@@ -4168,7 +4215,7 @@
         <v>20</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>90</v>
@@ -4183,28 +4230,28 @@
         <v>102</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4223,17 +4270,17 @@
         <v>91</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>20</v>
@@ -4282,7 +4329,7 @@
         <v>20</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
@@ -4297,28 +4344,28 @@
         <v>102</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4337,19 +4384,19 @@
         <v>91</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>20</v>
@@ -4398,7 +4445,7 @@
         <v>20</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
@@ -4413,28 +4460,28 @@
         <v>102</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
@@ -4453,19 +4500,19 @@
         <v>91</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>20</v>
@@ -4502,17 +4549,17 @@
         <v>20</v>
       </c>
       <c r="AB26" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AC26" s="2"/>
       <c r="AD26" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4527,30 +4574,30 @@
         <v>102</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
@@ -4569,19 +4616,19 @@
         <v>91</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>20</v>
@@ -4630,7 +4677,7 @@
         <v>20</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
@@ -4645,28 +4692,28 @@
         <v>102</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
@@ -4688,16 +4735,16 @@
         <v>125</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>20</v>
@@ -4746,7 +4793,7 @@
         <v>20</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -4764,25 +4811,25 @@
         <v>20</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
@@ -4801,19 +4848,19 @@
         <v>91</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>20</v>
@@ -4862,7 +4909,7 @@
         <v>20</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -4877,28 +4924,28 @@
         <v>102</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
@@ -4917,19 +4964,19 @@
         <v>91</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O30" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P30" t="s" s="2">
         <v>20</v>
@@ -4978,7 +5025,7 @@
         <v>20</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -4993,24 +5040,24 @@
         <v>102</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5018,7 +5065,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>79</v>
@@ -5033,19 +5080,19 @@
         <v>20</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>20</v>
@@ -5094,7 +5141,7 @@
         <v>20</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
@@ -5112,10 +5159,10 @@
         <v>20</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>20</v>
@@ -5123,14 +5170,14 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -5149,19 +5196,19 @@
         <v>20</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="O32" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>20</v>
@@ -5198,19 +5245,17 @@
         <v>20</v>
       </c>
       <c r="AB32" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC32" t="s" s="2">
-        <v>20</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="AC32" s="2"/>
       <c r="AD32" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5228,10 +5273,10 @@
         <v>20</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>20</v>
@@ -5239,21 +5284,23 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>320</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>331</v>
+      </c>
       <c r="D33" t="s" s="2">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>20</v>
@@ -5265,18 +5312,20 @@
         <v>20</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="O33" s="2"/>
+        <v>325</v>
+      </c>
+      <c r="O33" t="s" s="2">
+        <v>326</v>
+      </c>
       <c r="P33" t="s" s="2">
         <v>20</v>
       </c>
@@ -5324,7 +5373,7 @@
         <v>20</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
@@ -5342,10 +5391,10 @@
         <v>20</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>20</v>
+        <v>328</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>20</v>
@@ -5353,14 +5402,16 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="C34" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="B34" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
@@ -5376,20 +5427,22 @@
         <v>20</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="N34" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>325</v>
+      </c>
       <c r="O34" t="s" s="2">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>20</v>
@@ -5438,7 +5491,7 @@
         <v>20</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>78</v>
@@ -5450,16 +5503,16 @@
         <v>20</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>340</v>
+        <v>102</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>20</v>
@@ -5467,21 +5520,23 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="C35" s="2"/>
+        <v>320</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>337</v>
+      </c>
       <c r="D35" t="s" s="2">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>20</v>
@@ -5493,16 +5548,20 @@
         <v>20</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>104</v>
+        <v>323</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="O35" t="s" s="2">
+        <v>326</v>
+      </c>
       <c r="P35" t="s" s="2">
         <v>20</v>
       </c>
@@ -5550,28 +5609,28 @@
         <v>20</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>106</v>
+        <v>320</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>20</v>
+        <v>328</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>107</v>
+        <v>329</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>20</v>
@@ -5579,14 +5638,16 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>320</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>340</v>
+      </c>
       <c r="D36" t="s" s="2">
-        <v>109</v>
+        <v>321</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5605,18 +5666,20 @@
         <v>20</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>110</v>
+        <v>341</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>111</v>
+        <v>323</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>112</v>
+        <v>324</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="O36" s="2"/>
+        <v>325</v>
+      </c>
+      <c r="O36" t="s" s="2">
+        <v>326</v>
+      </c>
       <c r="P36" t="s" s="2">
         <v>20</v>
       </c>
@@ -5664,7 +5727,7 @@
         <v>20</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>117</v>
+        <v>320</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -5676,16 +5739,16 @@
         <v>20</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>20</v>
+        <v>328</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>107</v>
+        <v>329</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>20</v>
@@ -5693,14 +5756,14 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
-        <v>346</v>
+        <v>20</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s" s="2">
@@ -5713,26 +5776,24 @@
         <v>20</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>110</v>
+        <v>343</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="O37" t="s" s="2">
-        <v>195</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
         <v>20</v>
       </c>
@@ -5780,7 +5841,7 @@
         <v>20</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
@@ -5792,7 +5853,7 @@
         <v>20</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>20</v>
@@ -5801,7 +5862,7 @@
         <v>20</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>188</v>
+        <v>347</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>20</v>
@@ -5809,21 +5870,21 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>20</v>
+        <v>349</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>20</v>
@@ -5832,10 +5893,10 @@
         <v>20</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="L38" t="s" s="2">
         <v>351</v>
@@ -5843,11 +5904,9 @@
       <c r="M38" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="N38" t="s" s="2">
+      <c r="N38" s="2"/>
+      <c r="O38" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>20</v>
@@ -5896,28 +5955,28 @@
         <v>20</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>102</v>
+        <v>354</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>20</v>
+        <v>355</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>20</v>
@@ -5936,7 +5995,7 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>90</v>
@@ -5948,16 +6007,16 @@
         <v>20</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="K39" t="s" s="2">
         <v>357</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>358</v>
+        <v>104</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>359</v>
+        <v>105</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6008,10 +6067,10 @@
         <v>20</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>356</v>
+        <v>106</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>90</v>
@@ -6020,7 +6079,7 @@
         <v>20</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>20</v>
@@ -6029,7 +6088,7 @@
         <v>20</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>360</v>
+        <v>107</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>20</v>
@@ -6037,21 +6096,21 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>362</v>
+        <v>109</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>20</v>
@@ -6063,18 +6122,18 @@
         <v>20</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>343</v>
+        <v>110</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>363</v>
+        <v>111</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" t="s" s="2">
-        <v>365</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
         <v>20</v>
       </c>
@@ -6122,28 +6181,28 @@
         <v>20</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>361</v>
+        <v>117</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>366</v>
+        <v>20</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>367</v>
+        <v>107</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>20</v>
@@ -6151,14 +6210,14 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>20</v>
+        <v>360</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -6171,22 +6230,26 @@
         <v>20</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
+        <v>362</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="O41" t="s" s="2">
+        <v>195</v>
+      </c>
       <c r="P41" t="s" s="2">
         <v>20</v>
       </c>
@@ -6210,13 +6273,13 @@
         <v>20</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>371</v>
+        <v>20</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>372</v>
+        <v>20</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>20</v>
@@ -6234,7 +6297,7 @@
         <v>20</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>78</v>
@@ -6246,16 +6309,16 @@
         <v>20</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>366</v>
+        <v>20</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>373</v>
+        <v>188</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>20</v>
@@ -6263,10 +6326,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6277,7 +6340,7 @@
         <v>78</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>20</v>
@@ -6289,19 +6352,19 @@
         <v>20</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>20</v>
@@ -6350,13 +6413,13 @@
         <v>20</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>20</v>
@@ -6368,12 +6431,466 @@
         <v>20</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>366</v>
+        <v>20</v>
       </c>
       <c r="AM42" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="AN42" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="G43" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J43" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q43" s="2"/>
+      <c r="R43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AI43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AK43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL43" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM43" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AN43" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G44" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="L44" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="N44" s="2"/>
+      <c r="O44" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="P44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q44" s="2"/>
+      <c r="R44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF44" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="AG44" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH44" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AI44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AK44" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL44" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="AN42" t="s" s="2">
+      <c r="AM44" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="AN44" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G45" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q45" s="2"/>
+      <c r="R45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF45" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="AG45" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AK45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL45" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AM45" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="AN45" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G46" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K46" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="O46" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="P46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q46" s="2"/>
+      <c r="R46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AM46" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="AN46" t="s" s="2">
         <v>20</v>
       </c>
     </row>

</xml_diff>